<commit_message>
ignoring hidden files, adding data
</commit_message>
<xml_diff>
--- a/cms_system.xlsx
+++ b/cms_system.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C506BD-A0AC-5D4B-A734-884536D3A595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40868675-CDD1-4E4E-BA33-1B51409101B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28740" yWindow="4220" windowWidth="16860" windowHeight="20720" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Category</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Inner Tracker</t>
+  </si>
+  <si>
+    <t>Data (bytes)</t>
   </si>
 </sst>
 </file>
@@ -474,15 +477,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FF34C2-0233-224E-A21E-0372D088B6D7}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,13 +493,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -504,13 +510,17 @@
         <v>28</v>
       </c>
       <c r="C2">
+        <f>INT(1000000*E2)</f>
+        <v>1010000</v>
+      </c>
+      <c r="E2">
         <v>1.01</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>1.44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -518,13 +528,17 @@
         <v>5</v>
       </c>
       <c r="C3">
+        <f t="shared" ref="C3:C21" si="0">INT(1000000*E3)</f>
+        <v>500000</v>
+      </c>
+      <c r="E3">
         <v>0.5</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>0.72</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -532,13 +546,17 @@
         <v>6</v>
       </c>
       <c r="C4">
+        <f t="shared" si="0"/>
+        <v>300000</v>
+      </c>
+      <c r="E4">
         <v>0.3</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>0.43</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -546,13 +564,17 @@
         <v>7</v>
       </c>
       <c r="C5">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="E5">
         <v>0.01</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -560,13 +582,17 @@
         <v>9</v>
       </c>
       <c r="C6">
+        <f t="shared" si="0"/>
+        <v>170000</v>
+      </c>
+      <c r="E6">
         <v>0.17</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>0.24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -574,13 +600,17 @@
         <v>10</v>
       </c>
       <c r="C7">
+        <f t="shared" si="0"/>
+        <v>310000</v>
+      </c>
+      <c r="E7">
         <v>0.31</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>0.44</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -588,13 +618,17 @@
         <v>12</v>
       </c>
       <c r="C8">
+        <f t="shared" si="0"/>
+        <v>420000</v>
+      </c>
+      <c r="E8">
         <v>0.42</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -602,13 +636,17 @@
         <v>13</v>
       </c>
       <c r="C9">
+        <f t="shared" si="0"/>
+        <v>240000</v>
+      </c>
+      <c r="E9">
         <v>0.24</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>0.24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -616,13 +654,17 @@
         <v>14</v>
       </c>
       <c r="C10">
+        <f t="shared" si="0"/>
+        <v>30000</v>
+      </c>
+      <c r="E10">
         <v>0.03</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -630,13 +672,17 @@
         <v>15</v>
       </c>
       <c r="C11">
+        <f t="shared" si="0"/>
+        <v>60000</v>
+      </c>
+      <c r="E11">
         <v>0.06</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>0.06</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -644,13 +690,17 @@
         <v>16</v>
       </c>
       <c r="C12">
+        <f t="shared" si="0"/>
+        <v>2100000</v>
+      </c>
+      <c r="E12">
         <v>2.1</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -658,13 +708,17 @@
         <v>17</v>
       </c>
       <c r="C13">
+        <f t="shared" si="0"/>
+        <v>110000</v>
+      </c>
+      <c r="E13">
         <v>0.11</v>
       </c>
-      <c r="D13">
+      <c r="F13">
         <v>0.15</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -672,13 +726,17 @@
         <v>18</v>
       </c>
       <c r="C14">
+        <f t="shared" si="0"/>
+        <v>40000</v>
+      </c>
+      <c r="E14">
         <v>0.04</v>
       </c>
-      <c r="D14">
+      <c r="F14">
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -686,13 +744,17 @@
         <v>20</v>
       </c>
       <c r="C15">
+        <f t="shared" si="0"/>
+        <v>110000</v>
+      </c>
+      <c r="E15">
         <v>0.11</v>
       </c>
-      <c r="D15">
+      <c r="F15">
         <v>0.15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -700,13 +762,17 @@
         <v>21</v>
       </c>
       <c r="C16">
+        <f t="shared" si="0"/>
+        <v>330000</v>
+      </c>
+      <c r="E16">
         <v>0.33</v>
       </c>
-      <c r="D16">
+      <c r="F16">
         <v>0.47</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -714,13 +780,17 @@
         <v>22</v>
       </c>
       <c r="C17">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="E17">
         <v>2E-3</v>
       </c>
-      <c r="D17">
+      <c r="F17">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -728,13 +798,17 @@
         <v>23</v>
       </c>
       <c r="C18">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="E18">
         <v>1E-3</v>
       </c>
-      <c r="D18">
+      <c r="F18">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -742,13 +816,17 @@
         <v>24</v>
       </c>
       <c r="C19">
+        <f t="shared" si="0"/>
+        <v>80000</v>
+      </c>
+      <c r="E19">
         <v>0.08</v>
       </c>
-      <c r="D19">
+      <c r="F19">
         <v>0.12</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -756,13 +834,17 @@
         <v>25</v>
       </c>
       <c r="C20">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="E20">
         <v>0.01</v>
       </c>
-      <c r="D20">
+      <c r="F20">
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -770,9 +852,13 @@
         <v>27</v>
       </c>
       <c r="C21">
+        <f t="shared" si="0"/>
+        <v>260000</v>
+      </c>
+      <c r="E21">
         <v>0.26</v>
       </c>
-      <c r="D21">
+      <c r="F21">
         <v>0.26</v>
       </c>
     </row>

</xml_diff>